<commit_message>
add plots across TAL adsorbent capacity
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/TAL/analyses/current_state-system_TAL_adsorption_glucose-2022.4.11-22.34_5000sims_0_single_point.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/TAL/analyses/current_state-system_TAL_adsorption_glucose-2022.4.11-22.34_5000sims_0_single_point.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\TAL\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA611B37-10F8-4080-B649-9A693A7DCC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC48EBB3-7108-4173-A242-EE04B30F5195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,9 +309,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -321,6 +318,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -666,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK17"/>
+  <dimension ref="A1:BK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,82 +679,82 @@
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6" t="s">
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6" t="s">
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6" t="s">
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
+      <c r="BC1" s="10"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
     </row>
     <row r="2" spans="1:63" s="5" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1335,207 +1335,259 @@
       <c r="BF13" s="5"/>
     </row>
     <row r="14" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
       <c r="AB14" s="5"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
-      <c r="AF14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
       <c r="AL14" s="5"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="7"/>
-      <c r="AR14" s="7"/>
-      <c r="AS14" s="7"/>
-      <c r="AT14" s="7"/>
-      <c r="AU14" s="7"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="6"/>
       <c r="AV14" s="5"/>
-      <c r="AW14" s="7"/>
-      <c r="AX14" s="7"/>
-      <c r="AY14" s="7"/>
-      <c r="AZ14" s="7"/>
-      <c r="BB14" s="7"/>
-      <c r="BC14" s="7"/>
-      <c r="BD14" s="7"/>
-      <c r="BE14" s="7"/>
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="6"/>
+      <c r="AY14" s="6"/>
+      <c r="AZ14" s="6"/>
+      <c r="BB14" s="6"/>
+      <c r="BC14" s="6"/>
+      <c r="BD14" s="6"/>
+      <c r="BE14" s="6"/>
       <c r="BF14" s="5"/>
-      <c r="BG14" s="7"/>
-      <c r="BH14" s="7"/>
-      <c r="BI14" s="7"/>
-      <c r="BJ14" s="7"/>
+      <c r="BG14" s="6"/>
+      <c r="BH14" s="6"/>
+      <c r="BI14" s="6"/>
+      <c r="BJ14" s="6"/>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="7"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="7"/>
-      <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="7"/>
-      <c r="AQ15" s="7"/>
-      <c r="AR15" s="7"/>
-      <c r="AS15" s="7"/>
-      <c r="AT15" s="7"/>
-      <c r="AU15" s="7"/>
-      <c r="AV15" s="7"/>
-      <c r="AW15" s="7"/>
-      <c r="AX15" s="7"/>
-      <c r="AY15" s="7"/>
-      <c r="AZ15" s="7"/>
-      <c r="BA15" s="7"/>
-      <c r="BB15" s="7"/>
-      <c r="BC15" s="7"/>
-      <c r="BD15" s="7"/>
-      <c r="BE15" s="7"/>
-      <c r="BF15" s="7"/>
-      <c r="BG15" s="7"/>
-      <c r="BH15" s="7"/>
-      <c r="BI15" s="7"/>
-      <c r="BJ15" s="7"/>
-      <c r="BK15" s="7"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="6"/>
+      <c r="AP15" s="6"/>
+      <c r="AQ15" s="6"/>
+      <c r="AR15" s="6"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="6"/>
+      <c r="AU15" s="6"/>
+      <c r="AV15" s="6"/>
+      <c r="AW15" s="6"/>
+      <c r="AX15" s="6"/>
+      <c r="AY15" s="6"/>
+      <c r="AZ15" s="6"/>
+      <c r="BA15" s="6"/>
+      <c r="BB15" s="6"/>
+      <c r="BC15" s="6"/>
+      <c r="BD15" s="6"/>
+      <c r="BE15" s="6"/>
+      <c r="BF15" s="6"/>
+      <c r="BG15" s="6"/>
+      <c r="BH15" s="6"/>
+      <c r="BI15" s="6"/>
+      <c r="BJ15" s="6"/>
+      <c r="BK15" s="6"/>
     </row>
     <row r="16" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="8"/>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8"/>
-      <c r="AT16" s="8"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
-      <c r="AW16" s="8"/>
-      <c r="AX16" s="8"/>
-      <c r="AY16" s="8"/>
-      <c r="AZ16" s="8"/>
-      <c r="BA16" s="8"/>
-      <c r="BB16" s="8"/>
-      <c r="BC16" s="8"/>
-      <c r="BD16" s="8"/>
-      <c r="BE16" s="8"/>
-      <c r="BF16" s="8"/>
-      <c r="BG16" s="8"/>
-      <c r="BH16" s="8"/>
-      <c r="BI16" s="8"/>
-      <c r="BJ16" s="8"/>
-      <c r="BK16" s="8"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+      <c r="AO16" s="7"/>
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="7"/>
+      <c r="AR16" s="7"/>
+      <c r="AS16" s="7"/>
+      <c r="AT16" s="7"/>
+      <c r="AU16" s="7"/>
+      <c r="AV16" s="7"/>
+      <c r="AW16" s="7"/>
+      <c r="AX16" s="7"/>
+      <c r="AY16" s="7"/>
+      <c r="AZ16" s="7"/>
+      <c r="BA16" s="7"/>
+      <c r="BB16" s="7"/>
+      <c r="BC16" s="7"/>
+      <c r="BD16" s="7"/>
+      <c r="BE16" s="7"/>
+      <c r="BF16" s="7"/>
+      <c r="BG16" s="7"/>
+      <c r="BH16" s="7"/>
+      <c r="BI16" s="7"/>
+      <c r="BJ16" s="7"/>
+      <c r="BK16" s="7"/>
     </row>
-    <row r="17" spans="14:63" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="10"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
-      <c r="AJ17" s="10"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="10"/>
-      <c r="AN17" s="10"/>
-      <c r="AO17" s="10"/>
-      <c r="AP17" s="10"/>
-      <c r="AQ17" s="10"/>
-      <c r="AR17" s="10"/>
-      <c r="AS17" s="10"/>
-      <c r="AT17" s="10"/>
-      <c r="AU17" s="10"/>
-      <c r="AV17" s="10"/>
-      <c r="AW17" s="10"/>
-      <c r="AX17" s="10"/>
-      <c r="AY17" s="10"/>
-      <c r="AZ17" s="10"/>
-      <c r="BA17" s="10"/>
-      <c r="BB17" s="10"/>
-      <c r="BC17" s="10"/>
-      <c r="BD17" s="10"/>
-      <c r="BE17" s="10"/>
-      <c r="BF17" s="10"/>
-      <c r="BG17" s="10"/>
-      <c r="BH17" s="10"/>
-      <c r="BI17" s="10"/>
-      <c r="BJ17" s="10"/>
-      <c r="BK17" s="10"/>
+    <row r="17" spans="14:63" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
+      <c r="AN17" s="9"/>
+      <c r="AO17" s="9"/>
+      <c r="AP17" s="9"/>
+      <c r="AQ17" s="9"/>
+      <c r="AR17" s="9"/>
+      <c r="AS17" s="9"/>
+      <c r="AT17" s="9"/>
+      <c r="AU17" s="9"/>
+      <c r="AV17" s="9"/>
+      <c r="AW17" s="9"/>
+      <c r="AX17" s="9"/>
+      <c r="AY17" s="9"/>
+      <c r="AZ17" s="9"/>
+      <c r="BA17" s="9"/>
+      <c r="BB17" s="9"/>
+      <c r="BC17" s="9"/>
+      <c r="BD17" s="9"/>
+      <c r="BE17" s="9"/>
+      <c r="BF17" s="9"/>
+      <c r="BG17" s="9"/>
+      <c r="BH17" s="9"/>
+      <c r="BI17" s="9"/>
+      <c r="BJ17" s="9"/>
+      <c r="BK17" s="9"/>
+    </row>
+    <row r="18" spans="14:63" x14ac:dyDescent="0.3">
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="7"/>
+      <c r="AL18" s="7"/>
+      <c r="AM18" s="7"/>
+      <c r="AN18" s="7"/>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="7"/>
+      <c r="AR18" s="7"/>
+      <c r="AS18" s="7"/>
+      <c r="AT18" s="7"/>
+      <c r="AU18" s="7"/>
+      <c r="AV18" s="7"/>
+      <c r="AW18" s="7"/>
+      <c r="AX18" s="7"/>
+      <c r="AY18" s="7"/>
+      <c r="AZ18" s="7"/>
+      <c r="BA18" s="7"/>
+      <c r="BB18" s="7"/>
+      <c r="BC18" s="7"/>
+      <c r="BD18" s="7"/>
+      <c r="BE18" s="7"/>
+      <c r="BF18" s="7"/>
+      <c r="BG18" s="7"/>
+      <c r="BH18" s="7"/>
+      <c r="BI18" s="7"/>
+      <c r="BJ18" s="7"/>
+      <c r="BK18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>